<commit_message>
Update Equitas_Test Cases_20 May.xlsx
</commit_message>
<xml_diff>
--- a/Equitas_Test Cases_20 May.xlsx
+++ b/Equitas_Test Cases_20 May.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\JAY_JULY2024\TEST CASES\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sumedha\Workplace\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ED3125-B2FE-45D1-B163-048CC8FF8C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="20-MAY2025" sheetId="14" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Expected Behaviour</t>
   </si>
@@ -105,12 +104,15 @@
   </si>
   <si>
     <t>Doubtful</t>
+  </si>
+  <si>
+    <t>Transaction queue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,11 +596,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,7 +683,9 @@
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -874,14 +878,14 @@
       <c r="D34" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D80A67-091C-4E9F-8788-61F84F87902B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>